<commit_message>
add xlsxs and plankapy
</commit_message>
<xml_diff>
--- a/Umfrage_Phase1/Aufbereitet/Frage 2/Frage2Aufbereitet_16-18.xlsx
+++ b/Umfrage_Phase1/Aufbereitet/Frage 2/Frage2Aufbereitet_16-18.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Frage 2 Aufbereitet" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Rohdaten!$D$1:$D$21</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Rohdaten!$A$1:$AK$21</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -280,7 +280,7 @@
     <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
     <numFmt numFmtId="169" formatCode="0.00\ %"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +309,11 @@
       <name val="Aptos Narrow"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -416,11 +421,564 @@
       </fill>
     </dxf>
   </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFD320"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF579D1C"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Frage 2 Aufbereitet'!$A$3:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Instagram</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TikTok</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Snapchat</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Youtube</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Frage 2 Aufbereitet'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Frage 2 Aufbereitet'!$A$3:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Instagram</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TikTok</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Snapchat</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Youtube</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Frage 2 Aufbereitet'!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>38.7096774193548</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.5806451612903</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.45161290322581</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.258064516129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.728045502843928"/>
+          <c:y val="0.377930881209023"/>
+          <c:w val="0.12994562160135"/>
+          <c:h val="0.23235915101678"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>254520</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>55440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>324360</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>155520</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="2692800" y="380520"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -597,13 +1155,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AK21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F25" activeCellId="1" sqref="C3:C6 F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -721,7 +1279,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -807,7 +1365,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -881,7 +1439,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -958,7 +1516,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1035,7 +1593,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -1118,7 +1676,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -1195,7 +1753,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -1272,7 +1830,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -1358,7 +1916,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1429,7 +1987,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -1503,7 +2061,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1586,7 +2144,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1660,7 +2218,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -1746,7 +2304,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1820,7 +2378,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1894,7 +2452,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -1971,7 +2529,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
@@ -2069,7 +2627,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>70</v>
       </c>
@@ -2149,7 +2707,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
@@ -2238,7 +2796,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>70</v>
       </c>
@@ -2325,17 +2883,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D21">
-    <filterColumn colId="0" hiddenButton="1">
-      <filters>
-        <filter val=" 13 - 15"/>
-        <filter val=" 19 - 21"/>
-        <filter val="Jünger als 13"/>
-        <filter val="Älter als 21"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="0" hiddenButton="1"/>
-  </autoFilter>
+  <autoFilter ref="A1:AK21"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2355,7 +2903,7 @@
   <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2441,5 +2989,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;KffffffSeite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>